<commit_message>
adding sample input files and Excels
</commit_message>
<xml_diff>
--- a/input/estimator_template.xlsx
+++ b/input/estimator_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bhatramy/Desktop/Hadoop-estimator/framework/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bhatramy/Downloads/migration-effort-estimator/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C75B2A02-A313-B049-90A1-1C798B381C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4369513-5018-074D-A0B0-5197D0FCC89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,20 +23,11 @@
     <definedName name="Resource">Config!$M$2:$M$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t>Inventory and Characteristics</t>
   </si>
@@ -60,9 +51,6 @@
   </si>
   <si>
     <t>Conversion Type</t>
-  </si>
-  <si>
-    <t>Easy</t>
   </si>
   <si>
     <t>Medium</t>
@@ -591,7 +579,7 @@
   <dimension ref="B2:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -651,52 +639,52 @@
         <v>7</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="K3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B4" s="10"/>
       <c r="C4" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4">
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4" s="5">
         <v>4</v>
@@ -742,7 +730,7 @@
       <c r="B5" s="10"/>
       <c r="C5" s="9"/>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G5" s="5">
         <v>2</v>
@@ -788,7 +776,7 @@
       <c r="B6" s="10"/>
       <c r="C6" s="9"/>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6" s="5">
         <v>2</v>
@@ -834,7 +822,7 @@
       <c r="B7" s="10"/>
       <c r="C7" s="9"/>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G7" s="5">
         <v>2</v>
@@ -880,7 +868,7 @@
       <c r="B8" s="10"/>
       <c r="C8" s="9"/>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8" s="5">
         <v>2</v>
@@ -926,7 +914,7 @@
       <c r="B9" s="10"/>
       <c r="C9" s="9"/>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G9" s="5">
         <v>2</v>
@@ -972,7 +960,7 @@
       <c r="B10" s="10"/>
       <c r="C10" s="9"/>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G10" s="5">
         <v>2</v>
@@ -1061,22 +1049,22 @@
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="I1"/>
       <c r="J1"/>
@@ -1087,87 +1075,87 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="3">
         <v>0.5</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="F2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="3">
         <v>2</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="3">
         <v>3</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="G5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="3">
         <v>7</v>

</xml_diff>